<commit_message>
huge changes to pipeline - raw data is now in class structure and can be fed into a kilosort pipeline
</commit_message>
<xml_diff>
--- a/Adapter_pinout.xlsx
+++ b/Adapter_pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarlJ\Documents\_Python\CMU.43.004 Spike Sorting\Kilosort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DFFF2E-06DF-4628-8D4F-6D82F6D67955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6420E997-1451-4E7A-A135-69F06A65A44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CD1D033D-6F84-4F12-AEF8-A1E719ECA473}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>A32-Maps.pdf</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>(true)Intan Input</t>
+  </si>
+  <si>
+    <t>Intan Software Names</t>
   </si>
 </sst>
 </file>
@@ -2293,10 +2296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0245A86F-5F4F-41A2-B3BB-40002E4D2D97}">
-  <dimension ref="A3:S35"/>
+  <dimension ref="A3:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2316,9 +2319,10 @@
     <col min="13" max="13" width="7.140625" customWidth="1"/>
     <col min="14" max="14" width="4.42578125" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -2364,8 +2368,14 @@
       <c r="P3" s="5" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I4">
         <v>32</v>
       </c>
@@ -2381,12 +2391,12 @@
       <c r="P4" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="7"/>
-      <c r="S4" t="s">
+      <c r="T4" s="7"/>
+      <c r="U4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I5">
         <v>31</v>
       </c>
@@ -2403,7 +2413,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I6">
         <v>30</v>
       </c>
@@ -2420,7 +2430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I7">
         <v>29</v>
       </c>
@@ -2437,7 +2447,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I8">
         <v>28</v>
       </c>
@@ -2454,7 +2464,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I9">
         <v>27</v>
       </c>
@@ -2471,7 +2481,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I10">
         <v>26</v>
       </c>
@@ -2488,7 +2498,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I11">
         <v>25</v>
       </c>
@@ -2505,7 +2515,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I12">
         <v>24</v>
       </c>
@@ -2522,7 +2532,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I13">
         <v>23</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I14">
         <v>22</v>
       </c>
@@ -2556,7 +2566,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I15">
         <v>21</v>
       </c>
@@ -2573,7 +2583,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I16">
         <v>20</v>
       </c>
@@ -2924,10 +2934,10 @@
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4:O35">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P35">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>